<commit_message>
Updated report with images and some visual enhancement
</commit_message>
<xml_diff>
--- a/POPC/MATRIX/Parallel.xlsx
+++ b/POPC/MATRIX/Parallel.xlsx
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,22 +111,6 @@
       <color rgb="FF333333"/>
       <name val="Consolas"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -145,62 +129,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -223,61 +153,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2580,15 +2456,6 @@
       </c>
     </row>
     <row r="24" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>6240</v>
-      </c>
-      <c r="B24" s="2">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3</v>
-      </c>
       <c r="D24" s="2">
         <f>AVERAGE(D19:D23)</f>
         <v>6.5249159999999993</v>
@@ -2955,15 +2822,6 @@
       </c>
     </row>
     <row r="31" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>6240</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>2</v>
-      </c>
       <c r="D31" s="2">
         <f>AVERAGE(D26:D30)</f>
         <v>3.0271499999999998</v>
@@ -3216,15 +3074,6 @@
       </c>
     </row>
     <row r="38" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>6340</v>
-      </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2">
-        <v>2</v>
-      </c>
       <c r="D38" s="2">
         <f>AVERAGE(D33:D37)</f>
         <v>1.5941240000000003</v>
@@ -3813,15 +3662,6 @@
       </c>
     </row>
     <row r="47" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <v>4620</v>
-      </c>
-      <c r="B47" s="2">
-        <v>5</v>
-      </c>
-      <c r="C47" s="2">
-        <v>2</v>
-      </c>
       <c r="D47" s="2">
         <f>AVERAGE(D42:D46)</f>
         <v>9.1196520000000003</v>
@@ -4475,10 +4315,6 @@
         <f>AVERAGE(AG50:AG54)</f>
         <v>10.64772</v>
       </c>
-    </row>
-    <row r="56" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57"/>
@@ -4891,15 +4727,9 @@
       </c>
     </row>
     <row r="63" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>4620</v>
-      </c>
-      <c r="B63" s="2">
-        <v>2</v>
-      </c>
-      <c r="C63" s="2">
-        <v>3</v>
-      </c>
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
       <c r="D63" s="2">
         <f>AVERAGE(D58:D62)</f>
         <v>6.0681020000000006</v>
@@ -5302,15 +5132,9 @@
       </c>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
-        <v>4620</v>
-      </c>
-      <c r="B72" s="2">
-        <v>2</v>
-      </c>
-      <c r="C72" s="2">
-        <v>2</v>
-      </c>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
       <c r="D72" s="2">
         <f>AVERAGE(D67:D71)</f>
         <v>2.8609180000000003</v>
@@ -5611,15 +5435,9 @@
       </c>
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
-        <v>4620</v>
-      </c>
-      <c r="B79" s="2">
-        <v>1</v>
-      </c>
-      <c r="C79" s="2">
-        <v>2</v>
-      </c>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
       <c r="D79" s="2">
         <f>AVERAGE(D74:D78)</f>
         <v>1.33294</v>
@@ -6228,15 +6046,6 @@
       </c>
     </row>
     <row r="87" spans="1:36 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="2">
-        <v>3240</v>
-      </c>
-      <c r="B87" s="2">
-        <v>5</v>
-      </c>
-      <c r="C87" s="2">
-        <v>2</v>
-      </c>
       <c r="D87" s="2">
         <f>AVERAGE(D82:D86)</f>
         <v>8.9137140000000006</v>
@@ -6840,12 +6649,6 @@
         <f>AVERAGE(A89:A93)</f>
         <v>3240</v>
       </c>
-      <c r="B94" s="2">
-        <v>3</v>
-      </c>
-      <c r="C94" s="2">
-        <v>3</v>
-      </c>
       <c r="D94" s="2">
         <f>AVERAGE(D89:D93)</f>
         <v>8.2177159999999994</v>
@@ -6932,7 +6735,7 @@
       </c>
       <c r="XFD94" s="2">
         <f>AVERAGE(A94:XFC94)</f>
-        <v>139.60343741666671</v>
+        <v>152.02193172727277</v>
       </c>
     </row>
     <row r="95" spans="1:36 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7636,15 +7439,11 @@
       </c>
     </row>
     <row r="110" spans="1:29" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="2">
+      <c r="A110" s="1">
         <v>3240</v>
       </c>
-      <c r="B110" s="1">
-        <v>2</v>
-      </c>
-      <c r="C110" s="1">
-        <v>2</v>
-      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
       <c r="D110" s="2">
         <f>AVERAGE(D105:D109)</f>
         <v>2.7899479999999999</v>
@@ -7706,6 +7505,8 @@
       <c r="AC110" s="2"/>
     </row>
     <row r="111" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B111"/>
+      <c r="C111"/>
       <c r="D111"/>
       <c r="E111"/>
       <c r="F111"/>
@@ -7921,15 +7722,11 @@
       </c>
     </row>
     <row r="117" spans="1:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="2">
+      <c r="A117" s="1">
         <v>3240</v>
       </c>
-      <c r="B117" s="1">
-        <v>1</v>
-      </c>
-      <c r="C117" s="1">
-        <v>2</v>
-      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
       <c r="D117" s="2">
         <f>AVERAGE(D112:D116)</f>
         <v>1.3319459999999999</v>
@@ -7978,6 +7775,9 @@
       <c r="AB117" s="2"/>
       <c r="AC117" s="2"/>
     </row>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A118" s="2"/>
+    </row>
     <row r="122" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>2160</v>
@@ -8529,15 +8329,6 @@
       </c>
     </row>
     <row r="127" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="2">
-        <v>2160</v>
-      </c>
-      <c r="B127" s="2">
-        <v>5</v>
-      </c>
-      <c r="C127" s="2">
-        <v>2</v>
-      </c>
       <c r="D127" s="2">
         <f>AVERAGE(D122:D126)</f>
         <v>8.7300979999999999</v>
@@ -9137,15 +8928,6 @@
       </c>
     </row>
     <row r="134" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="2">
-        <v>2160</v>
-      </c>
-      <c r="B134" s="2">
-        <v>3</v>
-      </c>
-      <c r="C134" s="2">
-        <v>3</v>
-      </c>
       <c r="D134" s="2">
         <f>AVERAGE(D129:D133)</f>
         <v>8.1958859999999998</v>
@@ -9602,15 +9384,6 @@
       </c>
     </row>
     <row r="141" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="2">
-        <v>2160</v>
-      </c>
-      <c r="B141" s="2">
-        <v>2</v>
-      </c>
-      <c r="C141" s="2">
-        <v>3</v>
-      </c>
       <c r="D141" s="2">
         <f>AVERAGE(D136:D140)</f>
         <v>6.0317440000000007</v>
@@ -10215,15 +9988,6 @@
       </c>
     </row>
     <row r="155" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="2">
-        <v>2160</v>
-      </c>
-      <c r="B155" s="2">
-        <v>1</v>
-      </c>
-      <c r="C155" s="2">
-        <v>2</v>
-      </c>
       <c r="D155" s="2">
         <f>AVERAGE(D150:D154)</f>
         <v>1.3525680000000002</v>
@@ -10804,15 +10568,6 @@
       </c>
     </row>
     <row r="163" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="2">
-        <v>1080</v>
-      </c>
-      <c r="B163" s="2">
-        <v>5</v>
-      </c>
-      <c r="C163" s="2">
-        <v>2</v>
-      </c>
       <c r="D163" s="2">
         <f>AVERAGE(D158:D162)</f>
         <v>8.7312320000000003</v>
@@ -11412,15 +11167,6 @@
       </c>
     </row>
     <row r="170" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="2">
-        <v>1080</v>
-      </c>
-      <c r="B170" s="2">
-        <v>3</v>
-      </c>
-      <c r="C170" s="2">
-        <v>3</v>
-      </c>
       <c r="D170" s="2">
         <f>AVERAGE(D165:D169)</f>
         <v>8.1524759999999983</v>
@@ -11913,15 +11659,6 @@
       </c>
     </row>
     <row r="177" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="2">
-        <v>1080</v>
-      </c>
-      <c r="B177" s="2">
-        <v>2</v>
-      </c>
-      <c r="C177" s="2">
-        <v>3</v>
-      </c>
       <c r="D177" s="2">
         <f>AVERAGE(D172:D176)</f>
         <v>6.3635220000000006</v>
@@ -12287,16 +12024,7 @@
         <v>0.339613</v>
       </c>
     </row>
-    <row r="184" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A184" s="1">
-        <v>1080</v>
-      </c>
-      <c r="B184" s="1">
-        <v>2</v>
-      </c>
-      <c r="C184" s="1">
-        <v>2</v>
-      </c>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D184" s="2">
         <f>AVERAGE(D179:D183)</f>
         <v>2.7339500000000001</v>

</xml_diff>